<commit_message>
beta release  for workshop
</commit_message>
<xml_diff>
--- a/Materials/BOM-WeMakeColors.xlsx
+++ b/Materials/BOM-WeMakeColors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="700" windowWidth="25360" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>LED strip 9 LED</t>
   </si>
@@ -81,12 +81,6 @@
     <t>http://www.tme.eu/it/details/b2x25_bn330/bulloni/bossard/1122886/</t>
   </si>
   <si>
-    <t>B2X30/BN330</t>
-  </si>
-  <si>
-    <t>http://www.tme.eu/it/details/b2x30_bn330/bulloni/bossard/1122908/</t>
-  </si>
-  <si>
     <t>B2/BN628</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
   </si>
   <si>
     <t>screw 2ma 25mm</t>
-  </si>
-  <si>
-    <t>screw 2m 30mm</t>
   </si>
   <si>
     <t>DE</t>
@@ -602,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
@@ -619,22 +610,22 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>16</v>
@@ -643,13 +634,13 @@
         <v>17</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17" customHeight="1">
@@ -683,7 +674,7 @@
         <v>5.9383333333333335</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K3">
         <v>15</v>
@@ -720,7 +711,7 @@
         <v>1.1428571428571428</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" customHeight="1">
@@ -728,13 +719,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>150</v>
@@ -754,7 +745,7 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -762,10 +753,10 @@
     </row>
     <row r="6" spans="1:11" ht="17" customHeight="1">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
@@ -777,11 +768,11 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I14" si="1">G6*H6</f>
+        <f t="shared" ref="I6:I13" si="1">G6*H6</f>
         <v>3.75</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -792,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>14</v>
@@ -808,7 +799,7 @@
         <v>0.92</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -819,10 +810,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E8">
         <v>40</v>
@@ -842,7 +833,7 @@
         <v>0.66900000000000004</v>
       </c>
       <c r="J8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -853,10 +844,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>0.98</v>
@@ -869,7 +860,7 @@
         <v>0.98</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -880,10 +871,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G10">
         <v>2.2799999999999998</v>
@@ -896,7 +887,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="J10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K10">
         <v>7.9</v>
@@ -904,7 +895,7 @@
     </row>
     <row r="11" spans="1:11" ht="17" customHeight="1">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -917,94 +908,70 @@
         <v>2.64E-2</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>0.2112</v>
+        <v>0.36959999999999998</v>
       </c>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="17" customHeight="1">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G12">
-        <v>3.6299999999999999E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>0.1452</v>
+        <v>0.25</v>
       </c>
       <c r="J12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17" customHeight="1">
       <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="G13">
-        <v>1.2500000000000001E-2</v>
+        <v>2.7</v>
       </c>
       <c r="H13">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>0.22500000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="J13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="17" customHeight="1">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14">
-        <v>2.7</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>2.7</v>
-      </c>
-      <c r="J14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="17" customHeight="1">
-      <c r="H16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="5">
-        <f>SUM(I3:I14)</f>
-        <v>19.927590476190478</v>
-      </c>
-      <c r="K16" s="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="17" customHeight="1">
+      <c r="H15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="5">
+        <f>SUM(I3:I13)</f>
+        <v>19.965790476190474</v>
+      </c>
+      <c r="K15" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1012,12 +979,10 @@
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="D6" r:id="rId3"/>
     <hyperlink ref="D11" r:id="rId4"/>
-    <hyperlink ref="D12" r:id="rId5"/>
-    <hyperlink ref="D10" r:id="rId6"/>
-    <hyperlink ref="D14" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D13" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Support for FastLED library 3.1.6 and tested con core 2.4.0-rc2
</commit_message>
<xml_diff>
--- a/Materials/BOM-WeMakeColors.xlsx
+++ b/Materials/BOM-WeMakeColors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="3940" windowWidth="45680" windowHeight="22680" tabRatio="500"/>
+    <workbookView xWindow="1780" yWindow="560" windowWidth="42760" windowHeight="20160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bom 1.1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>LED strip 9 LED</t>
   </si>
@@ -221,16 +221,20 @@
   </si>
   <si>
     <t>http://it.aliexpress.com/item/Free-Shipping-400pcs-dupont-cable-jumper-wire-dupont-line-female-to-female-dupont-line-20cm-1P/1727878715.html</t>
+  </si>
+  <si>
+    <t>Price category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -272,6 +276,12 @@
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -321,7 +331,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -335,8 +345,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -359,20 +370,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -382,6 +397,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -717,7 +733,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
@@ -729,6 +745,7 @@
     <col min="5" max="5" width="8.83203125" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" customWidth="1"/>
     <col min="11" max="11" width="13.5" customWidth="1"/>
@@ -769,7 +786,7 @@
         <v>35</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>52</v>
@@ -788,17 +805,17 @@
       <c r="D3" s="17">
         <v>6</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="20">
         <v>35.630000000000003</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="29">
         <f>E3/D3</f>
         <v>5.9383333333333335</v>
       </c>
       <c r="G3" s="17">
         <v>1</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="20">
         <f>E3/D3</f>
         <v>5.9383333333333335</v>
       </c>
@@ -825,24 +842,24 @@
       <c r="D4" s="17">
         <v>7</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <v>8</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="29">
         <f>E4/D4</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="G4" s="17">
         <v>1</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="20">
         <f>E4/D4</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="20">
         <f>H3+H4</f>
         <v>7.0811904761904767</v>
       </c>
@@ -866,7 +883,7 @@
       <c r="E5" s="19">
         <v>16.100000000000001</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="30">
         <f>E5/D5</f>
         <v>0.10733333333333334</v>
       </c>
@@ -874,7 +891,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="19">
-        <f>F5*G5</f>
+        <f t="shared" ref="H5:H17" si="0">F5*G5</f>
         <v>0.96599999999999997</v>
       </c>
       <c r="I5" s="13" t="s">
@@ -895,14 +912,14 @@
         <v>24</v>
       </c>
       <c r="E6" s="19"/>
-      <c r="F6" s="23">
+      <c r="F6" s="30">
         <v>3.16</v>
       </c>
       <c r="G6" s="13">
         <v>1</v>
       </c>
       <c r="H6" s="19">
-        <f>F6*G6</f>
+        <f t="shared" si="0"/>
         <v>3.16</v>
       </c>
       <c r="I6" s="13" t="s">
@@ -928,7 +945,7 @@
       <c r="E7" s="19">
         <v>3.88</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="30">
         <f>E7/D7</f>
         <v>0.77600000000000002</v>
       </c>
@@ -936,7 +953,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="19">
-        <f>F7*G7</f>
+        <f t="shared" si="0"/>
         <v>0.77600000000000002</v>
       </c>
       <c r="I7" s="13" t="s">
@@ -962,7 +979,7 @@
       <c r="E8" s="19">
         <v>10.02</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="30">
         <f>E8/D8</f>
         <v>2.5049999999999999E-2</v>
       </c>
@@ -970,7 +987,7 @@
         <v>3</v>
       </c>
       <c r="H8" s="19">
-        <f>F8*G8</f>
+        <f t="shared" si="0"/>
         <v>7.5149999999999995E-2</v>
       </c>
       <c r="I8" s="13" t="s">
@@ -997,7 +1014,7 @@
       <c r="E9" s="19">
         <v>0.64</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="30">
         <f>E9/D9</f>
         <v>1.6E-2</v>
       </c>
@@ -1005,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="19">
-        <f>F9*G9</f>
+        <f t="shared" si="0"/>
         <v>1.6E-2</v>
       </c>
       <c r="I9" s="13" t="s">
@@ -1032,15 +1049,15 @@
       <c r="E10" s="10">
         <v>10.47</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="30">
         <f>E10/D10</f>
         <v>1.0470000000000002</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
       </c>
-      <c r="H10" s="26">
-        <f>F10*G10</f>
+      <c r="H10" s="23">
+        <f t="shared" si="0"/>
         <v>1.0470000000000002</v>
       </c>
       <c r="I10" s="10" t="s">
@@ -1066,24 +1083,24 @@
       <c r="E11" s="10">
         <v>13</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="31">
         <f>E11/D11</f>
         <v>1.3</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="26">
-        <f>F11*G11</f>
+      <c r="H11" s="23">
+        <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>36</v>
       </c>
       <c r="J11" s="10">
-        <v>7.9</v>
-      </c>
-      <c r="K11" s="26">
+        <v>0</v>
+      </c>
+      <c r="K11" s="23">
         <f>SUM(H5:H11)</f>
         <v>7.3401500000000004</v>
       </c>
@@ -1099,18 +1116,21 @@
         <v>16</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="25">
+      <c r="F12" s="32">
         <v>2.64E-2</v>
       </c>
       <c r="G12" s="5">
         <v>10</v>
       </c>
-      <c r="H12" s="22">
-        <f>F12*G12</f>
+      <c r="H12" s="21">
+        <f t="shared" si="0"/>
         <v>0.26400000000000001</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>37</v>
+      </c>
+      <c r="J12" s="5">
+        <v>7.9</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>17</v>
@@ -1123,14 +1143,14 @@
       <c r="B13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="32">
         <v>1.26E-2</v>
       </c>
       <c r="G13" s="5">
         <v>2</v>
       </c>
-      <c r="H13" s="22">
-        <f>F13*G13</f>
+      <c r="H13" s="21">
+        <f t="shared" si="0"/>
         <v>2.52E-2</v>
       </c>
       <c r="I13" s="5" t="s">
@@ -1147,14 +1167,14 @@
       <c r="B14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="32">
         <v>1.9400000000000001E-2</v>
       </c>
       <c r="G14" s="5">
         <v>2</v>
       </c>
-      <c r="H14" s="22">
-        <f>F14*G14</f>
+      <c r="H14" s="21">
+        <f t="shared" si="0"/>
         <v>3.8800000000000001E-2</v>
       </c>
       <c r="I14" s="5" t="s">
@@ -1172,14 +1192,14 @@
         <v>47</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="25">
+      <c r="F15" s="32">
         <v>0.11119999999999999</v>
       </c>
       <c r="G15" s="5">
         <v>2</v>
       </c>
-      <c r="H15" s="22">
-        <f>F15*G15</f>
+      <c r="H15" s="21">
+        <f t="shared" si="0"/>
         <v>0.22239999999999999</v>
       </c>
       <c r="I15" s="5" t="s">
@@ -1196,20 +1216,20 @@
       <c r="B16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="32">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="G16" s="5">
         <v>20</v>
       </c>
-      <c r="H16" s="22">
-        <f>F16*G16</f>
+      <c r="H16" s="21">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="21">
         <f>SUM(H12:H16)</f>
         <v>0.8004</v>
       </c>
@@ -1221,14 +1241,14 @@
       <c r="A17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="33">
         <v>2.7</v>
       </c>
       <c r="G17" s="8">
         <v>1</v>
       </c>
       <c r="H17" s="8">
-        <f>F17*G17</f>
+        <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
       <c r="I17" s="8" t="s">
@@ -1242,17 +1262,18 @@
       <c r="G19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="34">
         <f>SUM(H3:H17)</f>
         <v>17.921740476190479</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="K19">
+      <c r="K19" s="35">
         <f>SUM(K3:K17)</f>
         <v>15.221740476190476</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="H3:H8 H10:H16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
@@ -1349,8 +1370,8 @@
     <hyperlink ref="L9" r:id="rId9"/>
     <hyperlink ref="L10" r:id="rId10"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1421,13 +1442,13 @@
       <c r="B4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="22">
         <v>2.2799999999999998</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="23">
         <f t="shared" ref="H4" si="0">F4*G4</f>
         <v>2.2799999999999998</v>
       </c>
@@ -1458,14 +1479,14 @@
       <c r="E7" s="10">
         <v>10.47</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="22">
         <f>E7/D7</f>
         <v>1.0470000000000002</v>
       </c>
       <c r="G7" s="10">
         <v>1</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="23">
         <f t="shared" ref="H7" si="1">F7*G7</f>
         <v>1.0470000000000002</v>
       </c>
@@ -1479,20 +1500,20 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="27" customFormat="1" ht="17" customHeight="1">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:12" s="24" customFormat="1" ht="17" customHeight="1">
+      <c r="A9" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="H9" s="30"/>
-      <c r="L9" s="31"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="L9" s="28"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
@@ -1643,7 +1664,6 @@
     <hyperlink ref="L4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
led to show initial connection try to fix reconnect issue
</commit_message>
<xml_diff>
--- a/Materials/BOM-WeMakeColors.xlsx
+++ b/Materials/BOM-WeMakeColors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>LED strip 9 LED</t>
   </si>
@@ -100,9 +100,6 @@
     <t>http://it.aliexpress.com/item/1m-4m-5m-WS2812B-Smart-led-pixel-strip-Black-White-PCB-30-60-144-leds-m/2036819167.html?spm=2114.010208.3.1.WeGWPB&amp;ws_ab_test=searchweb201556_9,searchweb201644_3_505_506_503_504_10032_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_2,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=61284000-e116-4a69-8081-95e3a20c2009</t>
   </si>
   <si>
-    <t>White 5m 30 IP30</t>
-  </si>
-  <si>
     <t>Price parts</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>DE</t>
   </si>
   <si>
-    <t>20CM</t>
-  </si>
-  <si>
     <t>https://www.arduino.cc/en/Main/Donate</t>
   </si>
   <si>
@@ -214,9 +208,6 @@
     <t>http://it.aliexpress.com/item/Free-Shipping-5PCS-HC-SR501-Adjust-IR-Pyroelectric-Infrared-PIR-module-Motion-Sensor-Detector-Module/1766530570.html</t>
   </si>
   <si>
-    <t>10CM</t>
-  </si>
-  <si>
     <t>http://it.aliexpress.com/item/40pcs-lot-10cm-2-54mm-1pin-feMale-to-feMale-jumper-wire-Dupont-cable/32226515120.html</t>
   </si>
   <si>
@@ -224,6 +215,21 @@
   </si>
   <si>
     <t>Price category</t>
+  </si>
+  <si>
+    <t>WeMakeColors Bill of materials</t>
+  </si>
+  <si>
+    <t>White 3m flat</t>
+  </si>
+  <si>
+    <t>20 cm</t>
+  </si>
+  <si>
+    <t>10 cm</t>
+  </si>
+  <si>
+    <t>White 5 m 30 IP30</t>
   </si>
 </sst>
 </file>
@@ -733,13 +739,13 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" customWidth="1"/>
@@ -754,21 +760,21 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="17" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>14</v>
@@ -777,19 +783,19 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="17" customFormat="1" ht="17" customHeight="1">
@@ -820,7 +826,7 @@
         <v>5.9383333333333335</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="17">
         <v>15</v>
@@ -857,7 +863,7 @@
         <v>1.1428571428571428</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K4" s="20">
         <f>H3+H4</f>
@@ -872,10 +878,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="13">
         <v>150</v>
@@ -895,7 +901,7 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J5" s="13">
         <v>0</v>
@@ -923,13 +929,13 @@
         <v>3.16</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" s="13">
         <v>0</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="13" customFormat="1" ht="17" customHeight="1">
@@ -957,13 +963,13 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" s="13">
         <v>0</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="13" customFormat="1" ht="17" customHeight="1">
@@ -971,7 +977,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D8" s="13">
         <v>400</v>
@@ -991,14 +997,14 @@
         <v>7.5149999999999995E-2</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" s="13">
         <v>0</v>
       </c>
       <c r="K8" s="19"/>
       <c r="L8" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="13" customFormat="1" ht="17" customHeight="1">
@@ -1006,7 +1012,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D9" s="13">
         <v>40</v>
@@ -1026,14 +1032,14 @@
         <v>1.6E-2</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" s="13">
         <v>0</v>
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="10" customFormat="1" ht="17" customHeight="1">
@@ -1041,7 +1047,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D10" s="10">
         <v>10</v>
@@ -1061,13 +1067,13 @@
         <v>1.0470000000000002</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="10">
         <v>0</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="10" customFormat="1" ht="17" customHeight="1">
@@ -1075,7 +1081,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="10">
         <v>10</v>
@@ -1095,7 +1101,7 @@
         <v>1.3</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11" s="10">
         <v>0</v>
@@ -1105,12 +1111,12 @@
         <v>7.3401500000000004</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>16</v>
@@ -1127,7 +1133,7 @@
         <v>0.26400000000000001</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12" s="5">
         <v>7.9</v>
@@ -1138,10 +1144,10 @@
     </row>
     <row r="13" spans="1:12" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="A13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="F13" s="32">
         <v>1.26E-2</v>
@@ -1154,18 +1160,18 @@
         <v>2.52E-2</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" s="32">
         <v>1.9400000000000001E-2</v>
@@ -1178,18 +1184,18 @@
         <v>3.8800000000000001E-2</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="32">
@@ -1203,15 +1209,15 @@
         <v>0.22239999999999999</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>18</v>
@@ -1227,7 +1233,7 @@
         <v>0.25</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K16" s="21">
         <f>SUM(H12:H16)</f>
@@ -1252,15 +1258,15 @@
         <v>2.7</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" customHeight="1">
       <c r="G19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H19" s="34">
         <f>SUM(H3:H17)</f>
@@ -1371,7 +1377,6 @@
     <hyperlink ref="L10" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1396,22 +1401,22 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="17" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>14</v>
@@ -1420,19 +1425,19 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="10" customFormat="1" ht="17" customHeight="1">
@@ -1453,7 +1458,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="10">
         <v>7.9</v>
@@ -1471,7 +1476,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="10">
         <v>10</v>
@@ -1491,24 +1496,24 @@
         <v>1.0470000000000002</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" s="10">
         <v>0</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="24" customFormat="1" ht="17" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="26"/>

</xml_diff>